<commit_message>
update Result.xlsx  add new training mask_rcnn_R101_FPN_1x_coco2014_train_valminusmini add new testing data coco2014_minival git push
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -200,6 +200,12 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -216,12 +222,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -518,7 +518,7 @@
   <dimension ref="A3:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -614,10 +614,10 @@
       </c>
     </row>
     <row r="6" spans="1:10" s="8" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="17" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="6" t="s">
@@ -643,8 +643,8 @@
       </c>
     </row>
     <row r="7" spans="1:10" s="8" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="14"/>
-      <c r="C7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="18"/>
       <c r="D7" s="6" t="s">
         <v>12</v>
       </c>
@@ -774,10 +774,10 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="13" t="s">
         <v>2</v>
       </c>
       <c r="D12" s="4" t="s">
@@ -803,8 +803,8 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="18"/>
-      <c r="C13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="14"/>
       <c r="D13" s="4" t="s">
         <v>12</v>
       </c>
@@ -831,43 +831,67 @@
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="13" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
+      <c r="E14" s="10">
+        <v>0.30680000000000002</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0.52459999999999996</v>
+      </c>
+      <c r="G14" s="5">
+        <v>0.32040000000000002</v>
+      </c>
+      <c r="H14" s="5">
+        <v>0.1648</v>
+      </c>
+      <c r="I14" s="5">
+        <v>0.3402</v>
+      </c>
+      <c r="J14" s="5">
+        <v>0.40679999999999999</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="18"/>
-      <c r="C15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="14"/>
       <c r="D15" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
+      <c r="E15" s="1">
+        <v>0.27639999999999998</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.28089999999999998</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0.10970000000000001</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0.3024</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0.42020000000000002</v>
+      </c>
     </row>
     <row r="16" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="13" t="s">
         <v>2</v>
       </c>
       <c r="D16" s="9" t="s">
@@ -881,8 +905,8 @@
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" s="18"/>
-      <c r="C17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="14"/>
       <c r="D17" s="9" t="s">
         <v>12</v>
       </c>
@@ -895,11 +919,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C12:C13"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="B12:B13"/>
@@ -908,6 +927,11 @@
     <mergeCell ref="B8:B11"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="C10:C11"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C12:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
update Result.xlsx add new result iteration 180k
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -95,7 +95,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -173,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -199,6 +199,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -206,34 +221,22 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -518,16 +521,16 @@
   <dimension ref="A3:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.8984375" style="1"/>
-    <col min="2" max="2" width="26.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.8984375" style="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="26.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -560,10 +563,10 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -589,8 +592,8 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
       <c r="D5" s="3" t="s">
         <v>12</v>
       </c>
@@ -614,10 +617,10 @@
       </c>
     </row>
     <row r="6" spans="1:10" s="8" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="14" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="6" t="s">
@@ -643,8 +646,8 @@
       </c>
     </row>
     <row r="7" spans="1:10" s="8" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="16"/>
-      <c r="C7" s="18"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="15"/>
       <c r="D7" s="6" t="s">
         <v>12</v>
       </c>
@@ -668,10 +671,10 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="18" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -697,8 +700,8 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B9" s="21"/>
-      <c r="C9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="19"/>
       <c r="D9" s="3" t="s">
         <v>12</v>
       </c>
@@ -722,8 +725,8 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="21"/>
-      <c r="C10" s="22" t="s">
+      <c r="B10" s="20"/>
+      <c r="C10" s="21" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -749,8 +752,8 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="21"/>
-      <c r="C11" s="22"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="21"/>
       <c r="D11" s="3" t="s">
         <v>12</v>
       </c>
@@ -774,10 +777,10 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="22" t="s">
         <v>2</v>
       </c>
       <c r="D12" s="4" t="s">
@@ -803,8 +806,8 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="12"/>
-      <c r="C13" s="14"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="23"/>
       <c r="D13" s="4" t="s">
         <v>12</v>
       </c>
@@ -831,10 +834,10 @@
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="22" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="9" t="s">
@@ -860,27 +863,27 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="12"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="9" t="s">
+      <c r="B15" s="17"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="2">
         <v>0.27639999999999998</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="2">
         <v>0.48399999999999999</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="2">
         <v>0.28089999999999998</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="2">
         <v>0.10970000000000001</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I15" s="2">
         <v>0.3024</v>
       </c>
-      <c r="J15" s="1">
+      <c r="J15" s="2">
         <v>0.42020000000000002</v>
       </c>
     </row>
@@ -888,37 +891,66 @@
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="10"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
+      <c r="E16" s="10">
+        <v>0.33439999999999998</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="G16" s="5">
+        <v>0.35289999999999999</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0.17929999999999999</v>
+      </c>
+      <c r="I16" s="5">
+        <v>0.37019999999999997</v>
+      </c>
+      <c r="J16" s="5">
+        <v>0.4541</v>
+      </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" s="12"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="9" t="s">
+      <c r="B17" s="17"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="10"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
+      <c r="E17" s="2">
+        <v>0.2989</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0.51580000000000004</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0.30620000000000003</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0.1212</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0.3246</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0.46129999999999999</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C12:C13"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="B12:B13"/>
@@ -927,11 +959,6 @@
     <mergeCell ref="B8:B11"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="C10:C11"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C12:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
update result.xlsx iteration 270k
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="21">
   <si>
     <t>Train</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>iter 180k</t>
+  </si>
+  <si>
+    <t>iter 270k</t>
   </si>
 </sst>
 </file>
@@ -95,7 +98,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -173,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -202,6 +205,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -215,12 +233,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -231,12 +243,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -518,19 +524,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:J17"/>
+  <dimension ref="A3:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="26.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.8984375" style="1"/>
+    <col min="2" max="2" width="26.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.8984375" style="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -563,10 +569,10 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="21" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -592,8 +598,8 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
       <c r="D5" s="3" t="s">
         <v>12</v>
       </c>
@@ -617,10 +623,10 @@
       </c>
     </row>
     <row r="6" spans="1:10" s="8" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="19" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="6" t="s">
@@ -646,8 +652,8 @@
       </c>
     </row>
     <row r="7" spans="1:10" s="8" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="13"/>
-      <c r="C7" s="15"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="20"/>
       <c r="D7" s="6" t="s">
         <v>12</v>
       </c>
@@ -671,10 +677,10 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="21" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -700,8 +706,8 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B9" s="20"/>
-      <c r="C9" s="19"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="22"/>
       <c r="D9" s="3" t="s">
         <v>12</v>
       </c>
@@ -725,8 +731,8 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="20"/>
-      <c r="C10" s="21" t="s">
+      <c r="B10" s="23"/>
+      <c r="C10" s="24" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -752,8 +758,8 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="20"/>
-      <c r="C11" s="21"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="24"/>
       <c r="D11" s="3" t="s">
         <v>12</v>
       </c>
@@ -777,10 +783,10 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="15" t="s">
         <v>2</v>
       </c>
       <c r="D12" s="4" t="s">
@@ -806,8 +812,8 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="17"/>
-      <c r="C13" s="23"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="16"/>
       <c r="D13" s="4" t="s">
         <v>12</v>
       </c>
@@ -834,10 +840,10 @@
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="15" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="9" t="s">
@@ -863,8 +869,8 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="17"/>
-      <c r="C15" s="23"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="16"/>
       <c r="D15" s="11" t="s">
         <v>12</v>
       </c>
@@ -891,10 +897,10 @@
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="15" t="s">
         <v>2</v>
       </c>
       <c r="D16" s="11" t="s">
@@ -919,9 +925,9 @@
         <v>0.4541</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" s="17"/>
-      <c r="C17" s="23"/>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B17" s="14"/>
+      <c r="C17" s="16"/>
       <c r="D17" s="11" t="s">
         <v>12</v>
       </c>
@@ -944,13 +950,67 @@
         <v>0.46129999999999999</v>
       </c>
     </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="10">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0.57120000000000004</v>
+      </c>
+      <c r="G18" s="5">
+        <v>0.37019999999999997</v>
+      </c>
+      <c r="H18" s="5">
+        <v>0.193</v>
+      </c>
+      <c r="I18" s="5">
+        <v>0.3836</v>
+      </c>
+      <c r="J18" s="5">
+        <v>0.46879999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B19" s="14"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="10">
+        <v>0.30959999999999999</v>
+      </c>
+      <c r="F19" s="5">
+        <v>0.52929999999999999</v>
+      </c>
+      <c r="G19" s="5">
+        <v>0.3196</v>
+      </c>
+      <c r="H19" s="5">
+        <v>0.12939999999999999</v>
+      </c>
+      <c r="I19" s="5">
+        <v>0.3352</v>
+      </c>
+      <c r="J19" s="5">
+        <v>0.47870000000000001</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C12:C13"/>
+  <mergeCells count="15">
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="B12:B13"/>
@@ -959,6 +1019,11 @@
     <mergeCell ref="B8:B11"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="C10:C11"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C12:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
add training milestone in Result.xlsx
</commit_message>
<xml_diff>
--- a/Result.xlsx
+++ b/Result.xlsx
@@ -2,12 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Mask RCNN R100" sheetId="1" r:id="rId1"/>
+    <sheet name="training milestone" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
   <si>
     <t>Train</t>
   </si>
@@ -88,17 +89,77 @@
   </si>
   <si>
     <t>iter 270k</t>
+  </si>
+  <si>
+    <t>command</t>
+  </si>
+  <si>
+    <t>python tools/train_net.py \</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    --cfg configs/wattanapong/train_e2e_mask_rcnn_R-101-FPN_4x_coco2014_train_valminusmini_2gpu.yaml \</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    OUTPUT_DIR /tmp/detectron-output &gt; train_test_e2e_mask_rcnn_R-101-FPN_4x_coco2014_train_valminusmini_lr0_02.txt</t>
+  </si>
+  <si>
+    <t>tools</t>
+  </si>
+  <si>
+    <t>train_net.py</t>
+  </si>
+  <si>
+    <t>detectron</t>
+  </si>
+  <si>
+    <t>utils</t>
+  </si>
+  <si>
+    <t>train.py</t>
+  </si>
+  <si>
+    <t>train_model()</t>
+  </si>
+  <si>
+    <t>create_model()</t>
+  </si>
+  <si>
+    <t>detectron.utils.train.train_model()</t>
+  </si>
+  <si>
+    <t>checkpoint_iter</t>
+  </si>
+  <si>
+    <t>model_builder.create</t>
+  </si>
+  <si>
+    <t>modeling</t>
+  </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>Line</t>
+  </si>
+  <si>
+    <t>directory &amp; function</t>
+  </si>
+  <si>
+    <t>model_builder.py</t>
+  </si>
+  <si>
+    <t>create()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -109,7 +170,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -119,6 +180,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -176,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -242,6 +309,22 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -526,17 +609,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.8984375" style="1"/>
-    <col min="2" max="2" width="26.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.8984375" style="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="26.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1009,16 +1092,16 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C11"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C10:C11"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="B16:B17"/>
@@ -1028,4 +1111,181 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.77734375" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>110</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>50</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>98</v>
+      </c>
+      <c r="G10" s="25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>119</v>
+      </c>
+      <c r="H11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>134</v>
+      </c>
+      <c r="H12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>107</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="C6:M6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>